<commit_message>
Analyzed parameter space and changed code such that we can run differential_evolution many times and save the best parameters and see how close they are to each other. Furthermore tried to change strategy to randtobest1bin
</commit_message>
<xml_diff>
--- a/data/raw/TLiso.xlsx
+++ b/data/raw/TLiso.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrishadzimahovic/Desktop/DTU/6/Bachelor/MCLuminescence/data/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F62250-B8AE-F44C-9B9C-20994D85585B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA19CF12-8307-9C4B-A6FD-6BC1C957BBA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16820" activeTab="1" xr2:uid="{C8A70C76-2522-435E-9808-551DD02D62C5}"/>
   </bookViews>
@@ -3884,7 +3884,7 @@
   <dimension ref="A1:O22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>